<commit_message>
Results with domains as binomial outcome,Age revised to 60 and above
</commit_message>
<xml_diff>
--- a/Table 3.xlsx
+++ b/Table 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\PhD-Study-IV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD71BD0D-F6D4-437E-AFD1-00C986347F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9272BA0-E9B9-4F25-A612-71EADEC3E3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B83F6E9B-6BE5-41D6-878E-8B219F79BD93}"/>
   </bookViews>
@@ -36,21 +36,9 @@
     <t>Male 18-32 years</t>
   </si>
   <si>
-    <t>Male 33-49 years</t>
-  </si>
-  <si>
-    <t>Male 50 years and above</t>
-  </si>
-  <si>
     <t>Female 18-32 years</t>
   </si>
   <si>
-    <t>Female 33-49 years</t>
-  </si>
-  <si>
-    <t>Female 50 years and above</t>
-  </si>
-  <si>
     <t>Mobility</t>
   </si>
   <si>
@@ -66,9 +54,6 @@
     <t>Anxiety/Depression</t>
   </si>
   <si>
-    <t>SD</t>
-  </si>
-  <si>
     <t>Percentage</t>
   </si>
   <si>
@@ -79,6 +64,21 @@
   </si>
   <si>
     <t>*Percentage reporting any problems</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Female 60 years and above</t>
+  </si>
+  <si>
+    <t>Male 60 years and above</t>
+  </si>
+  <si>
+    <t>Male 33-59 years</t>
+  </si>
+  <si>
+    <t>Female 33-59 years</t>
   </si>
 </sst>
 </file>
@@ -161,35 +161,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +510,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,238 +524,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="6">
+        <v>84.4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="D3" s="13">
+        <v>45.2</v>
+      </c>
+      <c r="E3" s="13">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F3" s="13">
+        <v>56.8</v>
+      </c>
+      <c r="G3" s="13">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="H3" s="13">
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
+        <v>79.2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.27</v>
+      </c>
+      <c r="D4" s="14">
+        <v>39.29</v>
+      </c>
+      <c r="E4" s="15">
+        <v>30.8</v>
+      </c>
+      <c r="F4" s="15">
+        <v>50.76</v>
+      </c>
+      <c r="G4" s="15">
+        <v>55.3</v>
+      </c>
+      <c r="H4" s="15">
+        <v>34.880000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="B5" s="12">
+        <v>79.8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5.28</v>
+      </c>
+      <c r="D5" s="16">
+        <v>51.28</v>
+      </c>
+      <c r="E5" s="15">
+        <v>39.1</v>
+      </c>
+      <c r="F5" s="15">
+        <v>63.01</v>
+      </c>
+      <c r="G5" s="15">
+        <v>71.23</v>
+      </c>
+      <c r="H5" s="15">
+        <v>50.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10">
-        <v>76.8</v>
-      </c>
-      <c r="C3" s="10">
-        <v>20.5</v>
-      </c>
-      <c r="D3" s="10">
-        <v>45.2</v>
-      </c>
-      <c r="E3" s="10">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="F3" s="10">
-        <v>56.8</v>
-      </c>
-      <c r="G3" s="10">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="H3" s="10">
-        <v>41.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8">
-        <v>79.2</v>
-      </c>
-      <c r="C4" s="5">
-        <v>20.57</v>
-      </c>
-      <c r="D4" s="11">
-        <v>39.29</v>
-      </c>
-      <c r="E4" s="12">
-        <v>30.8</v>
-      </c>
-      <c r="F4" s="12">
-        <v>50.76</v>
-      </c>
-      <c r="G4" s="12">
-        <v>55.3</v>
-      </c>
-      <c r="H4" s="12">
-        <v>34.880000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="12">
+        <v>82</v>
+      </c>
+      <c r="C6" s="4">
+        <v>20.22</v>
+      </c>
+      <c r="D6" s="16">
+        <v>47.61</v>
+      </c>
+      <c r="E6" s="15">
+        <v>38.090000000000003</v>
+      </c>
+      <c r="F6" s="15">
+        <v>56.1</v>
+      </c>
+      <c r="G6" s="15">
+        <v>72.03</v>
+      </c>
+      <c r="H6" s="15">
+        <v>37.14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15">
-        <v>73.12</v>
-      </c>
-      <c r="C5" s="6">
-        <v>21.7</v>
-      </c>
-      <c r="D5" s="7">
-        <v>51.28</v>
-      </c>
-      <c r="E5" s="13">
-        <v>39.1</v>
-      </c>
-      <c r="F5" s="17">
-        <v>63.01</v>
-      </c>
-      <c r="G5" s="13">
-        <v>71.23</v>
-      </c>
-      <c r="H5" s="17">
-        <v>50.69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6">
-        <v>74.83</v>
-      </c>
-      <c r="C6" s="6">
-        <v>20.22</v>
-      </c>
-      <c r="D6" s="7">
-        <v>47.61</v>
-      </c>
-      <c r="E6" s="13">
-        <v>38.090000000000003</v>
-      </c>
-      <c r="F6" s="13">
-        <v>56.1</v>
-      </c>
-      <c r="G6" s="13">
-        <v>72.03</v>
-      </c>
-      <c r="H6" s="13">
-        <v>37.14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8">
-        <v>80.45</v>
-      </c>
-      <c r="C7" s="6">
-        <v>15.02</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="B7" s="17">
+        <v>85</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5.27</v>
+      </c>
+      <c r="D7" s="14">
         <v>44.4</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="15">
         <v>37.03</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="15">
         <v>59.25</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="15">
         <v>68.510000000000005</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="15">
         <v>46.2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="15">
-        <v>72.760000000000005</v>
-      </c>
-      <c r="C8" s="6">
-        <v>26.25</v>
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="12">
+        <v>82.7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4.9000000000000004</v>
       </c>
       <c r="D8" s="16">
         <v>51.28</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="9">
         <v>48.71</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="9">
         <v>66.67</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="15">
         <v>71.790000000000006</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="9">
         <v>61.53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6">
-        <v>78.290000000000006</v>
-      </c>
-      <c r="C9" s="6">
-        <v>16.25</v>
-      </c>
-      <c r="D9" s="16">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12">
+        <v>81.8</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5.86</v>
+      </c>
+      <c r="D9" s="8">
         <v>51.85</v>
       </c>
       <c r="E9" s="16">
         <v>44.44</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="16">
         <v>62.96</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="8">
         <v>75.92</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="16">
         <v>47.05</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>17</v>
+      <c r="A10" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised Statistics, Results, & first draft Discussion
</commit_message>
<xml_diff>
--- a/Table 3.xlsx
+++ b/Table 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\PhD-Study-IV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9272BA0-E9B9-4F25-A612-71EADEC3E3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAC5280-0E83-4FAD-8BB7-9521FF6524A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B83F6E9B-6BE5-41D6-878E-8B219F79BD93}"/>
   </bookViews>
@@ -178,12 +178,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -193,6 +187,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +524,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
@@ -548,7 +548,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
@@ -576,24 +576,24 @@
         <v>10</v>
       </c>
       <c r="B3" s="6">
-        <v>84.4</v>
+        <v>81.75</v>
       </c>
       <c r="C3" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="D3" s="13">
+        <v>7.8</v>
+      </c>
+      <c r="D3" s="11">
         <v>45.2</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>36.799999999999997</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="11">
         <v>56.8</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="11">
         <v>65.599999999999994</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>41.1</v>
       </c>
     </row>
@@ -601,25 +601,25 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>79.2</v>
       </c>
       <c r="C4" s="3">
         <v>5.27</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>39.29</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <v>30.8</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>50.76</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="13">
         <v>55.3</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <v>34.880000000000003</v>
       </c>
     </row>
@@ -627,25 +627,25 @@
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>79.8</v>
       </c>
       <c r="C5" s="4">
         <v>5.28</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="14">
         <v>51.28</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="13">
         <v>39.1</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="13">
         <v>63.01</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="13">
         <v>71.23</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="13">
         <v>50.69</v>
       </c>
     </row>
@@ -653,25 +653,25 @@
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>82</v>
       </c>
       <c r="C6" s="4">
         <v>20.22</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="14">
         <v>47.61</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <v>38.090000000000003</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="13">
         <v>56.1</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="13">
         <v>72.03</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="13">
         <v>37.14</v>
       </c>
     </row>
@@ -679,25 +679,25 @@
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="15">
         <v>85</v>
       </c>
       <c r="C7" s="4">
         <v>5.27</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>44.4</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <v>37.03</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <v>59.25</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>68.510000000000005</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="13">
         <v>46.2</v>
       </c>
     </row>
@@ -705,13 +705,13 @@
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>82.7</v>
       </c>
       <c r="C8" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="14">
         <v>51.28</v>
       </c>
       <c r="E8" s="9">
@@ -720,7 +720,7 @@
       <c r="F8" s="9">
         <v>66.67</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>71.790000000000006</v>
       </c>
       <c r="H8" s="9">
@@ -731,7 +731,7 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>81.8</v>
       </c>
       <c r="C9" s="4">
@@ -740,16 +740,16 @@
       <c r="D9" s="8">
         <v>51.85</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="14">
         <v>44.44</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <v>62.96</v>
       </c>
       <c r="G9" s="8">
         <v>75.92</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="14">
         <v>47.05</v>
       </c>
     </row>

</xml_diff>